<commit_message>
Updated FIN_grids model - 2025-08-25 18:19
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_FIN_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FIN_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10DCAFC9-4F24-43E2-B46E-BAAA5B4643B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11911F43-CCEE-458B-A835-0E67F5E7FEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVA" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="174">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -112,18 +112,9 @@
     <t>io</t>
   </si>
   <si>
-    <t>ELC_Sol*</t>
-  </si>
-  <si>
-    <t>ELC_Win*</t>
-  </si>
-  <si>
     <t>IN</t>
   </si>
   <si>
-    <t>~TFM_FILL-R: w=weo_pg; hcol=year</t>
-  </si>
-  <si>
     <t>attribute</t>
   </si>
   <si>
@@ -232,6 +223,36 @@
     <t>allregions</t>
   </si>
   <si>
+    <t>ELC_spv*</t>
+  </si>
+  <si>
+    <t>ELC_won*</t>
+  </si>
+  <si>
+    <t>Trd_elec*</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>pset_ci</t>
+  </si>
+  <si>
+    <t>solar,wind,coal,gas,nuclear,hydro</t>
+  </si>
+  <si>
+    <t>attrib_cond</t>
+  </si>
+  <si>
+    <t>-pasti</t>
+  </si>
+  <si>
     <t>~replicateinregions</t>
   </si>
   <si>
@@ -244,19 +265,301 @@
     <t>FIN</t>
   </si>
   <si>
-    <t>FI1-220</t>
+    <t>w53047196-400</t>
+  </si>
+  <si>
+    <t>at grid node - w53047196-400</t>
   </si>
   <si>
     <t>Bioenergy + CCUS,Bioenergy - Large scale unit,CCGT,CCGT + CCS,Coal + CCS,Gas turbine,IGCC,IGCC + CCS,Nuclear large,Oxyfuel + CCS,Steam Coal - SUBCRITICAL,Steam Coal - SUPERCRITICAL,Steam Coal - ULTRASUPERCRITICAL</t>
   </si>
   <si>
+    <t>w98609844-400</t>
+  </si>
+  <si>
+    <t>at grid node - w98609844-400</t>
+  </si>
+  <si>
+    <t>FI15-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI15-400</t>
+  </si>
+  <si>
+    <t>w34623113-400</t>
+  </si>
+  <si>
+    <t>at grid node - w34623113-400</t>
+  </si>
+  <si>
+    <t>w1306874220-400</t>
+  </si>
+  <si>
+    <t>at grid node - w1306874220-400</t>
+  </si>
+  <si>
+    <t>FI37-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI37-400</t>
+  </si>
+  <si>
+    <t>w28820749-400</t>
+  </si>
+  <si>
+    <t>at grid node - w28820749-400</t>
+  </si>
+  <si>
+    <t>w498816162-400</t>
+  </si>
+  <si>
+    <t>at grid node - w498816162-400</t>
+  </si>
+  <si>
+    <t>w151818544-400</t>
+  </si>
+  <si>
+    <t>at grid node - w151818544-400</t>
+  </si>
+  <si>
+    <t>w55275882-400</t>
+  </si>
+  <si>
+    <t>at grid node - w55275882-400</t>
+  </si>
+  <si>
+    <t>w150209972-400</t>
+  </si>
+  <si>
+    <t>at grid node - w150209972-400</t>
+  </si>
+  <si>
     <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by vision · Guided by intuition · Fueled by passion</t>
   </si>
   <si>
+    <t>w98561229-400</t>
+  </si>
+  <si>
+    <t>at grid node - w98561229-400</t>
+  </si>
+  <si>
     <t>EN_Hydro_FIN-1,EN_Hydro_FIN-2,EN_Hydro_FIN-3</t>
   </si>
   <si>
+    <t>w47317827-400</t>
+  </si>
+  <si>
+    <t>at grid node - w47317827-400</t>
+  </si>
+  <si>
+    <t>w388832477-220</t>
+  </si>
+  <si>
+    <t>at grid node - w388832477-220</t>
+  </si>
+  <si>
+    <t>w286955409-220</t>
+  </si>
+  <si>
+    <t>at grid node - w286955409-220</t>
+  </si>
+  <si>
+    <t>w388655178-400</t>
+  </si>
+  <si>
+    <t>at grid node - w388655178-400</t>
+  </si>
+  <si>
+    <t>w149965738-220</t>
+  </si>
+  <si>
+    <t>at grid node - w149965738-220</t>
+  </si>
+  <si>
+    <t>FI2-220</t>
+  </si>
+  <si>
+    <t>at grid node - FI2-220</t>
+  </si>
+  <si>
+    <t>w169899622-220</t>
+  </si>
+  <si>
+    <t>at grid node - w169899622-220</t>
+  </si>
+  <si>
+    <t>w55609623-220</t>
+  </si>
+  <si>
+    <t>at grid node - w55609623-220</t>
+  </si>
+  <si>
     <t>EN_STG8hbNREL,EN_STG4hbNREL</t>
+  </si>
+  <si>
+    <t>w43143343-400</t>
+  </si>
+  <si>
+    <t>at grid node - w43143343-400</t>
+  </si>
+  <si>
+    <t>w144832705-400</t>
+  </si>
+  <si>
+    <t>at grid node - w144832705-400</t>
+  </si>
+  <si>
+    <t>FI38-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI38-400</t>
+  </si>
+  <si>
+    <t>w128463750-400</t>
+  </si>
+  <si>
+    <t>at grid node - w128463750-400</t>
+  </si>
+  <si>
+    <t>w98735006-400</t>
+  </si>
+  <si>
+    <t>at grid node - w98735006-400</t>
+  </si>
+  <si>
+    <t>w26619335</t>
+  </si>
+  <si>
+    <t>at grid node - w26619335</t>
+  </si>
+  <si>
+    <t>w208979069-400</t>
+  </si>
+  <si>
+    <t>at grid node - w208979069-400</t>
+  </si>
+  <si>
+    <t>w1155254820-400</t>
+  </si>
+  <si>
+    <t>at grid node - w1155254820-400</t>
+  </si>
+  <si>
+    <t>w1107461441-400</t>
+  </si>
+  <si>
+    <t>at grid node - w1107461441-400</t>
+  </si>
+  <si>
+    <t>w1286130176-400</t>
+  </si>
+  <si>
+    <t>at grid node - w1286130176-400</t>
+  </si>
+  <si>
+    <t>w881741424-400</t>
+  </si>
+  <si>
+    <t>at grid node - w881741424-400</t>
+  </si>
+  <si>
+    <t>w544156119-400</t>
+  </si>
+  <si>
+    <t>at grid node - w544156119-400</t>
+  </si>
+  <si>
+    <t>w136068907-400</t>
+  </si>
+  <si>
+    <t>at grid node - w136068907-400</t>
+  </si>
+  <si>
+    <t>w123462491-400</t>
+  </si>
+  <si>
+    <t>at grid node - w123462491-400</t>
+  </si>
+  <si>
+    <t>w551596913-400</t>
+  </si>
+  <si>
+    <t>at grid node - w551596913-400</t>
+  </si>
+  <si>
+    <t>w351960012-220</t>
+  </si>
+  <si>
+    <t>at grid node - w351960012-220</t>
+  </si>
+  <si>
+    <t>w1321685855-400</t>
+  </si>
+  <si>
+    <t>at grid node - w1321685855-400</t>
+  </si>
+  <si>
+    <t>FI8-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI8-400</t>
+  </si>
+  <si>
+    <t>w590767557-400</t>
+  </si>
+  <si>
+    <t>at grid node - w590767557-400</t>
+  </si>
+  <si>
+    <t>w1275744419</t>
+  </si>
+  <si>
+    <t>at grid node - w1275744419</t>
+  </si>
+  <si>
+    <t>FI13-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI13-400</t>
+  </si>
+  <si>
+    <t>e_demand,ev_battery,H2prd_Elc_PEM,H2prd_Elc_ALK</t>
+  </si>
+  <si>
+    <t>FI26-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI26-400</t>
+  </si>
+  <si>
+    <t>FI34-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI34-400</t>
+  </si>
+  <si>
+    <t>FI4-400</t>
+  </si>
+  <si>
+    <t>at grid node - FI4-400</t>
+  </si>
+  <si>
+    <t>w159532385-400</t>
+  </si>
+  <si>
+    <t>at grid node - w159532385-400</t>
+  </si>
+  <si>
+    <t>w35281467-400</t>
+  </si>
+  <si>
+    <t>at grid node - w35281467-400</t>
+  </si>
+  <si>
+    <t>w98613134-400</t>
+  </si>
+  <si>
+    <t>at grid node - w98613134-400</t>
   </si>
 </sst>
 </file>
@@ -374,16 +677,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,8 +716,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>296862</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
@@ -421,7 +726,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58481C18-4BC2-E525-041C-7A7733EDDCD7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10139C99-125E-0F45-B4F4-374076437E35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -719,140 +1024,1117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268E9BAB-B98F-4B82-9042-51EABC9ED525}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="4" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.59765625" customWidth="1"/>
-    <col min="7" max="9" width="10.59765625" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.46484375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.59765625" customWidth="1"/>
-    <col min="12" max="14" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" customWidth="1"/>
+    <col min="13" max="13" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.06640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.59765625" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.46484375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="5" t="s">
+    <row r="9" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="5" t="s">
+      <c r="G10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="O10" s="5" t="s">
+      <c r="L10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="O11" s="6" t="s">
+      <c r="Q10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="6" t="s">
         <v>72</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="B16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="B17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="B18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="B19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="B20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="S20" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="T20" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="B21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R22" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="S22" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="T22" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="T24" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="S26" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="T26" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L27" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L31" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="L32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="O32" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L33" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M34" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L35" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L37" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O38" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L39" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L41" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L42" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M42" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="N42" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="O42" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L44" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M44" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="N44" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L45" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L46" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="N46" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="O46" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L47" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L48" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M48" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="O48" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L49" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N49" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="12:15" x14ac:dyDescent="0.45">
+      <c r="L50" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N50" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O50" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -868,9 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3954DD3-0F24-46DF-B268-7A98442D0282}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -891,13 +2171,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -906,69 +2186,69 @@
         <v>22</v>
       </c>
       <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>43</v>
-      </c>
-      <c r="M1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L2">
         <v>2700</v>
@@ -980,42 +2260,42 @@
         <v>2700</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L3">
         <v>1110</v>
@@ -1027,42 +2307,42 @@
         <v>480</v>
       </c>
       <c r="O3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" t="s">
-        <v>51</v>
-      </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L4">
         <v>4060</v>
@@ -1074,42 +2354,42 @@
         <v>1980</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>51</v>
-      </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L5">
         <v>1500</v>
@@ -1121,42 +2401,42 @@
         <v>1370</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L6">
         <v>70</v>
@@ -1168,42 +2448,42 @@
         <v>65</v>
       </c>
       <c r="O6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
-      </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L7">
         <v>16</v>
@@ -1215,42 +2495,42 @@
         <v>16</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L8">
         <v>120</v>
@@ -1262,42 +2542,42 @@
         <v>70</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" t="s">
-        <v>51</v>
-      </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L9">
         <v>38</v>
@@ -1309,42 +2589,42 @@
         <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -1356,42 +2636,42 @@
         <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L11">
         <v>1.5</v>
@@ -1403,42 +2683,42 @@
         <v>1.5</v>
       </c>
       <c r="O11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L12">
         <v>3</v>
@@ -1450,42 +2730,42 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L13">
         <v>1.5</v>
@@ -1497,7 +2777,7 @@
         <v>1.5</v>
       </c>
       <c r="O13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1507,10 +2787,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C3:X41"/>
+  <dimension ref="C4:X48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1527,20 +2807,15 @@
     <col min="14" max="14" width="4.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:24" x14ac:dyDescent="0.45">
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s">
         <v>21</v>
@@ -1563,13 +2838,13 @@
         <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="3:24" x14ac:dyDescent="0.45">
@@ -1577,19 +2852,19 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1">
         <v>8.76</v>
       </c>
       <c r="L6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.45">
@@ -1597,19 +2872,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G7">
         <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.45">
@@ -1617,7 +2892,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -1639,29 +2914,38 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G10">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="1">
+        <v>8.76</v>
+      </c>
       <c r="P11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="3:24" x14ac:dyDescent="0.45">
       <c r="P12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T12" t="s">
         <v>21</v>
@@ -1672,7 +2956,7 @@
         <v>4</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q13" s="2">
         <v>2700</v>
@@ -1688,7 +2972,7 @@
         <v>EN[_]Hydro*</v>
       </c>
       <c r="W13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="X13" t="s">
         <v>19</v>
@@ -1711,7 +2995,7 @@
         <v>5</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q14" s="2">
         <v>1110</v>
@@ -1727,10 +3011,10 @@
         <v>E[_]SPV*</v>
       </c>
       <c r="W14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="X14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="3:24" x14ac:dyDescent="0.45">
@@ -1741,7 +3025,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1750,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q15" s="2">
         <v>4060</v>
@@ -1766,10 +3050,10 @@
         <v>E[_]WOF*</v>
       </c>
       <c r="W15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="X15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="3:24" x14ac:dyDescent="0.45">
@@ -1777,13 +3061,13 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G16" s="1">
         <v>8.76</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q16" s="2">
         <v>1500</v>
@@ -1799,10 +3083,10 @@
         <v>E[_]WON*</v>
       </c>
       <c r="W16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="X16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="3:24" x14ac:dyDescent="0.45">
@@ -1810,13 +3094,13 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G17">
         <v>4</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q17" s="2">
         <v>70</v>
@@ -1845,13 +3129,13 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q18" s="2">
         <v>16</v>
@@ -1880,13 +3164,13 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G19">
         <v>30</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q19" s="2">
         <v>120</v>
@@ -1915,13 +3199,13 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q20" s="2">
         <v>38</v>
@@ -1956,7 +3240,7 @@
         <v>0.25</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q21" s="2">
         <v>4</v>
@@ -1985,13 +3269,13 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G22">
         <v>20</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q22" s="2">
         <v>1.5</v>
@@ -2017,7 +3301,7 @@
     </row>
     <row r="23" spans="3:24" x14ac:dyDescent="0.45">
       <c r="P23" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q23" s="2">
         <v>3</v>
@@ -2043,7 +3327,7 @@
     </row>
     <row r="24" spans="3:24" x14ac:dyDescent="0.45">
       <c r="P24" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q24" s="2">
         <v>1.5</v>
@@ -2102,7 +3386,7 @@
     </row>
     <row r="30" spans="3:24" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -2190,10 +3474,10 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" t="s">
         <v>24</v>
-      </c>
-      <c r="E40" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.45">
@@ -2201,10 +3485,65 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
         <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48">
+        <v>2025</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>